<commit_message>
Addition of some regional aircrafts
</commit_message>
<xml_diff>
--- a/ComputeCapacity/AirplaneData.xlsx
+++ b/ComputeCapacity/AirplaneData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edgar\Google Drive (nexelane@gmail.com)\Technologies and studies_\Planes\Aerodynamics\Simulations\INITIALSIZING-Aeros\ComputeCapacity\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{14FCAA11-5926-4360-9F5B-A4C70D986EE1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFB8961B-DCE8-4B52-B281-00D863801E19}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{3C58E045-F2D5-44A3-ADD5-F060913E18FE}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="34">
   <si>
     <t>g</t>
   </si>
@@ -117,6 +117,21 @@
   </si>
   <si>
     <t>MF</t>
+  </si>
+  <si>
+    <t>Batt Vol. Ratio</t>
+  </si>
+  <si>
+    <t>Fuel Vol.ratio</t>
+  </si>
+  <si>
+    <t>Fuel V*</t>
+  </si>
+  <si>
+    <t>Batt Vol*</t>
+  </si>
+  <si>
+    <t>Wh/l</t>
   </si>
 </sst>
 </file>
@@ -221,7 +236,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
@@ -240,6 +255,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -556,20 +574,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{66F40615-F021-408E-ACCC-D84F8BF2777F}">
-  <dimension ref="B2:O42"/>
+  <dimension ref="B2:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="14.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14.33203125" customWidth="1"/>
+    <col min="11" max="11" width="14.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="2" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="G2" s="5" t="s">
         <v>19</v>
       </c>
@@ -959,617 +982,782 @@
         <v>27</v>
       </c>
     </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>13</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D15" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H15" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L15" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
     <row r="16" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C16" s="11" t="s">
+      <c r="B16">
+        <v>14</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L16" s="1">
+        <v>2000</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="O16" s="4"/>
+    </row>
+    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C18" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D16" s="12"/>
-      <c r="E16" s="13"/>
-      <c r="G16" s="5" t="s">
+      <c r="D18" s="12"/>
+      <c r="E18" s="13"/>
+      <c r="G18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="H16" s="6"/>
-      <c r="I16" s="7"/>
-      <c r="K16" s="5" t="s">
+      <c r="H18" s="12"/>
+      <c r="I18" s="13"/>
+      <c r="K18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="L16" s="6"/>
-      <c r="M16" s="7"/>
-      <c r="O16" s="4"/>
-    </row>
-    <row r="17" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C17" s="1" t="s">
+      <c r="L18" s="12"/>
+      <c r="M18" s="13"/>
+    </row>
+    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D19" s="1">
         <f>6.6</f>
         <v>6.6</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="H17" s="1">
+      <c r="H19" s="1">
         <v>16.466000000000001</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I19" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="L17" s="1">
+      <c r="L19" s="1">
         <v>38.6</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="M19" s="1" t="s">
         <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D18" s="1">
-        <v>19.98</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H18" s="2">
-        <f>SQRT(H24*H27)</f>
-        <v>27.399270063269935</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="K18" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="L18" s="1">
-        <v>26</v>
-      </c>
-      <c r="M18" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="19" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D19" s="1">
-        <v>9.8070000000000004</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="1">
-        <v>9.8070000000000004</v>
-      </c>
-      <c r="I19" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="K19" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="L19" s="1">
-        <v>9.8070000000000004</v>
-      </c>
-      <c r="M19" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="20" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D20" s="1">
-        <f>(D17*D19)</f>
-        <v>64.726200000000006</v>
+        <v>19.98</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H20" s="1">
-        <f>(H17*H19)</f>
-        <v>161.48206200000001</v>
+        <v>4</v>
+      </c>
+      <c r="H20" s="2">
+        <f>SQRT(H26*H29)</f>
+        <v>27.399270063269935</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="L20" s="1">
-        <f>(L17*L19)</f>
-        <v>378.55020000000002</v>
+        <v>26</v>
       </c>
       <c r="M20" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D21" s="1">
+        <v>9.8070000000000004</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="1">
+        <v>9.8070000000000004</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="L21" s="1">
+        <v>9.8070000000000004</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22" s="1">
+        <f>(D19*D21)</f>
+        <v>64.726200000000006</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H22" s="1">
+        <f>(H19*H21)</f>
+        <v>161.48206200000001</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K22" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="L22" s="1">
+        <f>(L19*L21)</f>
+        <v>378.55020000000002</v>
+      </c>
+      <c r="M22" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D23" s="1">
         <v>112.5</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H21" s="2">
+      <c r="H23" s="2">
         <f>535/3.6</f>
         <v>148.61111111111111</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I23" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L21" s="2">
+      <c r="L23" s="2">
         <f>871/3.6</f>
         <v>241.94444444444443</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="M23" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="22" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D22" s="1">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H22" s="1">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="K22" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="L22" s="1">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="M22" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="23" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D23" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E23" s="1"/>
-      <c r="G23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="I23" s="1"/>
-      <c r="K23" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="L23" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="M23" s="1"/>
     </row>
     <row r="24" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D24" s="2">
-        <f>(D18^2)/D27</f>
-        <v>11.451531841652324</v>
-      </c>
-      <c r="E24" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="G24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H24" s="2">
-        <v>13.8</v>
-      </c>
-      <c r="I24" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="H24" s="1">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="I24" s="1" t="s">
+        <v>15</v>
+      </c>
       <c r="K24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="L24" s="2">
-        <f>(L18^2)/L27</f>
-        <v>9.2933736596095695</v>
-      </c>
-      <c r="M24" s="1"/>
+        <v>7</v>
+      </c>
+      <c r="L24" s="1">
+        <v>0.60399999999999998</v>
+      </c>
+      <c r="M24" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="25" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C25" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D25" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.8</v>
       </c>
       <c r="E25" s="1"/>
       <c r="G25" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="H25" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.8</v>
       </c>
       <c r="I25" s="1"/>
       <c r="K25" s="1" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L25" s="1">
-        <v>2.1999999999999999E-2</v>
+        <v>0.8</v>
       </c>
       <c r="M25" s="1"/>
     </row>
     <row r="26" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D26" s="1">
-        <v>1.5</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="D26" s="2">
+        <f>(D20^2)/D29</f>
+        <v>11.451531841652324</v>
+      </c>
+      <c r="E26" s="1"/>
       <c r="G26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="1">
-        <v>2.0840000000000001</v>
-      </c>
-      <c r="I26" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="H26" s="2">
+        <v>13.8</v>
+      </c>
+      <c r="I26" s="1"/>
       <c r="K26" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="L26" s="1">
-        <v>3.9820000000000002</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>25</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="L26" s="2">
+        <f>(L20^2)/L29</f>
+        <v>9.2933736596095695</v>
+      </c>
+      <c r="M26" s="1"/>
     </row>
     <row r="27" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="G27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H27" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I27" s="1"/>
+      <c r="K27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="L27" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="M27" s="1"/>
+    </row>
+    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D28" s="1">
+        <v>1.5</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H28" s="1">
+        <v>2.0840000000000001</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="K28" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="L28" s="1">
+        <v>3.9820000000000002</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="N28" s="4"/>
+    </row>
+    <row r="29" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D29" s="1">
         <v>34.86</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G27" s="1" t="s">
+      <c r="G29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H27" s="1">
+      <c r="H29" s="1">
         <v>54.4</v>
       </c>
-      <c r="I27" s="1" t="s">
+      <c r="I29" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="K27" s="1" t="s">
+      <c r="K29" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="L27" s="8">
+      <c r="L29" s="8">
         <v>72.739999999999995</v>
       </c>
-      <c r="M27" s="1" t="s">
+      <c r="M29" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="28" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C28" s="9" t="s">
+    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
+      <c r="C30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D30" s="1">
         <v>1.3</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G28" s="9" t="s">
+      <c r="G30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H28" s="1">
+      <c r="H30" s="1">
         <v>4.3890000000000002</v>
       </c>
-      <c r="I28" s="1" t="s">
+      <c r="I30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="K28" s="9" t="s">
+      <c r="K30" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="L28" s="1">
+      <c r="L30" s="1">
         <v>7.6340000000000003</v>
       </c>
-      <c r="M28" s="1" t="s">
+      <c r="M30" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="N28" s="4"/>
-    </row>
-    <row r="30" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C30" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D30" s="12"/>
-      <c r="E30" s="13"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="H30" s="6"/>
-      <c r="I30" s="7"/>
     </row>
     <row r="31" spans="3:14" x14ac:dyDescent="0.3">
-      <c r="C31" s="1" t="s">
-        <v>26</v>
+      <c r="C31" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="D31" s="1">
-        <v>20.100000000000001</v>
+        <v>10000</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G31" s="1" t="s">
-        <v>26</v>
+        <v>33</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>30</v>
       </c>
       <c r="H31" s="1">
-        <v>21.5</v>
+        <v>10000</v>
       </c>
       <c r="I31" s="1" t="s">
-        <v>10</v>
+        <v>33</v>
+      </c>
+      <c r="K31" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="L31" s="1">
+        <v>10000</v>
+      </c>
+      <c r="M31" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="3:14" x14ac:dyDescent="0.3">
       <c r="C32" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="D32" s="1">
-        <v>20.04</v>
+        <v>2000</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>11</v>
+        <v>33</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="H32" s="1">
-        <v>24.51</v>
+        <v>2000</v>
       </c>
       <c r="I32" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D33" s="1">
-        <v>9.8070000000000004</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H33" s="1">
-        <v>9.8070000000000004</v>
-      </c>
-      <c r="I33" s="1" t="s">
-        <v>12</v>
+        <v>33</v>
+      </c>
+      <c r="K32" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L32" s="1">
+        <v>2000</v>
+      </c>
+      <c r="M32" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D34" s="1">
-        <f>(D31*D33)</f>
-        <v>197.12070000000003</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="G34" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H34" s="1">
-        <f>(H31*H33)</f>
-        <v>210.85050000000001</v>
-      </c>
-      <c r="I34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="L34" s="4"/>
+      <c r="C34" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D34" s="12"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="H34" s="12"/>
+      <c r="I34" s="13"/>
     </row>
     <row r="35" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D35" s="1">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="H35" s="1">
+        <v>21.5</v>
+      </c>
+      <c r="I35" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D36" s="1">
+        <v>20.04</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H36" s="1">
+        <v>24.51</v>
+      </c>
+      <c r="I36" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="L36" s="4"/>
+    </row>
+    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D37" s="1">
+        <v>9.8070000000000004</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="H37" s="1">
+        <v>9.8070000000000004</v>
+      </c>
+      <c r="I37" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D38" s="1">
+        <f>(D35*D37)</f>
+        <v>197.12070000000003</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G38" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="1">
+        <f>(H35*H37)</f>
+        <v>210.85050000000001</v>
+      </c>
+      <c r="I38" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D35" s="2">
+      <c r="D39" s="2">
         <f>833/3.6</f>
         <v>231.38888888888889</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="E39" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G35" s="1" t="s">
+      <c r="G39" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="2">
+      <c r="H39" s="2">
         <f>460/3.6</f>
         <v>127.77777777777777</v>
       </c>
-      <c r="I35" s="1" t="s">
+      <c r="I39" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="36" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D36" s="1">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="H36" s="1">
-        <v>0.60399999999999998</v>
-      </c>
-      <c r="I36" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D37" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="E37" s="1"/>
-      <c r="G37" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37" s="1">
-        <v>0.8</v>
-      </c>
-      <c r="I37" s="1"/>
-    </row>
-    <row r="38" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D38" s="2">
-        <f>(D32^2)/D41</f>
-        <v>7.8437812499999993</v>
-      </c>
-      <c r="E38" s="1"/>
-      <c r="G38" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H38" s="2">
-        <f>(H32^2)/H41</f>
-        <v>11.779217647058825</v>
-      </c>
-      <c r="I38" s="1"/>
-    </row>
-    <row r="39" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D39" s="1">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="E39" s="1"/>
-      <c r="G39" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H39" s="1">
-        <v>2.1999999999999999E-2</v>
-      </c>
-      <c r="I39" s="1"/>
     </row>
     <row r="40" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C40" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D40" s="1">
-        <v>2.3199999999999998</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="H40" s="1">
-        <v>3.68</v>
+        <v>0.60399999999999998</v>
       </c>
       <c r="I40" s="1" t="s">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="41" spans="3:12" x14ac:dyDescent="0.3">
       <c r="C41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="E41" s="1"/>
+      <c r="G41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41" s="1">
+        <v>0.8</v>
+      </c>
+      <c r="I41" s="1"/>
+    </row>
+    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D42" s="2">
+        <f>(D36^2)/D45</f>
+        <v>7.8437812499999993</v>
+      </c>
+      <c r="E42" s="1"/>
+      <c r="G42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H42" s="2">
+        <f>(H36^2)/H45</f>
+        <v>11.779217647058825</v>
+      </c>
+      <c r="I42" s="1"/>
+    </row>
+    <row r="43" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E43" s="1"/>
+      <c r="G43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H43" s="1">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="I43" s="1"/>
+    </row>
+    <row r="44" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D44" s="1">
+        <v>2.3199999999999998</v>
+      </c>
+      <c r="E44" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G44" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H44" s="1">
+        <v>3.68</v>
+      </c>
+      <c r="I44" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D45" s="1">
         <v>51.2</v>
       </c>
-      <c r="E41" s="1" t="s">
+      <c r="E45" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="G41" s="1" t="s">
+      <c r="G45" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H41" s="1">
+      <c r="H45" s="1">
         <v>51</v>
       </c>
-      <c r="I41" s="1" t="s">
+      <c r="I45" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="42" spans="3:12" x14ac:dyDescent="0.3">
-      <c r="C42" s="9" t="s">
+    <row r="46" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C46" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D46" s="1">
         <v>4.17</v>
       </c>
-      <c r="E42" s="1" t="s">
+      <c r="E46" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G42" s="9" t="s">
+      <c r="G46" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="H42" s="10">
+      <c r="H46" s="10">
         <v>4.4400000000000004</v>
       </c>
-      <c r="I42" s="1" t="s">
+      <c r="I46" s="1" t="s">
         <v>27</v>
       </c>
     </row>
+    <row r="47" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C47" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D47" s="1">
+        <v>10000</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="H47" s="1">
+        <v>10000</v>
+      </c>
+      <c r="I47" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="3:12" x14ac:dyDescent="0.3">
+      <c r="C48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D48" s="8">
+        <v>2000</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H48" s="8">
+        <v>2000</v>
+      </c>
+      <c r="I48" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C30:E30"/>
+  <mergeCells count="6">
+    <mergeCell ref="K18:M18"/>
     <mergeCell ref="C2:E2"/>
-    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="G34:I34"/>
+    <mergeCell ref="G18:I18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" r:id="rId1"/>

</xml_diff>